<commit_message>
Convert NameConversions to use the new list of syntax
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/NameConversions.xlsx
+++ b/SampleTests/ExcelTests/NameConversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{999888BC-410E-4983-864E-AE00F13BE5A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D2DE38D4-B93C-4788-B43C-2AABACF90452}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Specification</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Anything</t>
   </si>
   <si>
-    <t>List_Property(0) of</t>
-  </si>
-  <si>
     <t>Do_Nothing</t>
   </si>
   <si>
@@ -95,6 +92,12 @@
   </si>
   <si>
     <t>Underscores in names are converted to underscores in C#, it just checks that the code compiles, and doesn't contain any meaningful setup or assertions.</t>
+  </si>
+  <si>
+    <t>List_Property list of</t>
+  </si>
+  <si>
+    <t>With Item</t>
   </si>
 </sst>
 </file>
@@ -1507,13 +1510,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1521,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1531,7 +1534,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,7 +1542,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1549,7 +1552,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1663,7 +1666,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,13 +1687,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1716,15 +1719,15 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1737,10 +1740,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,7 +1766,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,7 +1776,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Record root classes distinctly
Root class should always be generated, and in a slightly different way
to classes that mimic things in the sut, so highlighting them as
different paves the way for this
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/NameConversions.xlsx
+++ b/SampleTests/ExcelTests/NameConversions.xlsx
@@ -1515,8 +1515,10 @@
       <x:c r="B1" s="1" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C1" t="s">
-        <x:v>22</x:v>
+      <x:c r="C1" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
       </x:c>
       <x:c r="F1" s="1" t="s">
         <x:v>6</x:v>

</xml_diff>